<commit_message>
AP: energy is added to pion qT data
</commit_message>
<xml_diff>
--- a/pion_qT/expdata/1001.xlsx
+++ b/pion_qT/expdata/1001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninacao/Desktop/fitpack2/database/pion_qT/expdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avp5627/GIT/fitpack2/database/pion_qT/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5643BC-CC37-0943-9ED6-65E80FBFBF1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D316DA3-9BB7-4B4A-A274-9ECE3E169BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{E6E3B163-33F6-E044-A176-E8F274F71224}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="17040" xr2:uid="{E6E3B163-33F6-E044-A176-E8F274F71224}"/>
   </bookViews>
   <sheets>
     <sheet name="d2sigma dpTdm" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="16">
   <si>
     <t>m_min</t>
   </si>
@@ -76,6 +79,9 @@
   </si>
   <si>
     <t>%norm_c</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -290,7 +296,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -588,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F3B301-59A3-0B41-A64A-DE11E6B1716B}">
   <dimension ref="A1:S156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="P157" sqref="P157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,6 +640,9 @@
       <c r="K1" s="16" t="s">
         <v>14</v>
       </c>
+      <c r="L1" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="S1" s="17"/>
     </row>
     <row r="2" spans="1:19" ht="17" x14ac:dyDescent="0.25">
@@ -671,6 +680,9 @@
       <c r="K2" s="15">
         <v>16</v>
       </c>
+      <c r="L2" s="15">
+        <v>252</v>
+      </c>
       <c r="S2" s="17"/>
     </row>
     <row r="3" spans="1:19" ht="17" x14ac:dyDescent="0.25">
@@ -708,6 +720,9 @@
       <c r="K3" s="15">
         <v>16</v>
       </c>
+      <c r="L3" s="15">
+        <v>252</v>
+      </c>
       <c r="S3" s="17"/>
     </row>
     <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.25">
@@ -745,6 +760,9 @@
       <c r="K4" s="15">
         <v>16</v>
       </c>
+      <c r="L4" s="15">
+        <v>252</v>
+      </c>
       <c r="S4" s="17"/>
     </row>
     <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.25">
@@ -782,6 +800,9 @@
       <c r="K5" s="15">
         <v>16</v>
       </c>
+      <c r="L5" s="15">
+        <v>252</v>
+      </c>
       <c r="S5" s="17"/>
     </row>
     <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.25">
@@ -819,6 +840,9 @@
       <c r="K6" s="15">
         <v>16</v>
       </c>
+      <c r="L6" s="15">
+        <v>252</v>
+      </c>
       <c r="S6" s="17"/>
     </row>
     <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -856,6 +880,9 @@
       <c r="K7" s="15">
         <v>16</v>
       </c>
+      <c r="L7" s="15">
+        <v>252</v>
+      </c>
     </row>
     <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
@@ -892,6 +919,9 @@
       <c r="K8" s="15">
         <v>16</v>
       </c>
+      <c r="L8" s="15">
+        <v>252</v>
+      </c>
       <c r="S8" s="17"/>
     </row>
     <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.25">
@@ -929,6 +959,9 @@
       <c r="K9" s="15">
         <v>16</v>
       </c>
+      <c r="L9" s="15">
+        <v>252</v>
+      </c>
       <c r="S9" s="17"/>
     </row>
     <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -966,6 +999,9 @@
       <c r="K10" s="15">
         <v>16</v>
       </c>
+      <c r="L10" s="15">
+        <v>252</v>
+      </c>
     </row>
     <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
@@ -1002,6 +1038,9 @@
       <c r="K11" s="15">
         <v>16</v>
       </c>
+      <c r="L11" s="15">
+        <v>252</v>
+      </c>
     </row>
     <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
@@ -1038,6 +1077,9 @@
       <c r="K12" s="15">
         <v>16</v>
       </c>
+      <c r="L12" s="15">
+        <v>252</v>
+      </c>
     </row>
     <row r="13" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
@@ -1074,6 +1116,9 @@
       <c r="K13" s="15">
         <v>16</v>
       </c>
+      <c r="L13" s="15">
+        <v>252</v>
+      </c>
     </row>
     <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
@@ -1110,6 +1155,9 @@
       <c r="K14" s="15">
         <v>16</v>
       </c>
+      <c r="L14" s="15">
+        <v>252</v>
+      </c>
     </row>
     <row r="15" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
@@ -1146,6 +1194,9 @@
       <c r="K15" s="15">
         <v>16</v>
       </c>
+      <c r="L15" s="15">
+        <v>252</v>
+      </c>
     </row>
     <row r="16" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
@@ -1182,8 +1233,11 @@
       <c r="K16" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L16" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -1218,8 +1272,11 @@
       <c r="K17" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L17" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -1254,8 +1311,11 @@
       <c r="K18" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L18" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -1290,8 +1350,11 @@
       <c r="K19" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L19" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -1326,8 +1389,11 @@
       <c r="K20" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L20" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -1362,8 +1428,11 @@
       <c r="K21" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L21" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -1398,8 +1467,11 @@
       <c r="K22" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L22" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -1434,8 +1506,11 @@
       <c r="K23" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L23" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -1470,8 +1545,11 @@
       <c r="K24" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L24" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -1506,8 +1584,11 @@
       <c r="K25" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L25" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -1542,8 +1623,11 @@
       <c r="K26" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L26" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -1578,8 +1662,11 @@
       <c r="K27" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L27" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -1614,8 +1701,11 @@
       <c r="K28" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L28" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -1650,8 +1740,11 @@
       <c r="K29" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L29" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -1686,8 +1779,11 @@
       <c r="K30" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L30" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -1722,8 +1818,11 @@
       <c r="K31" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L31" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -1758,8 +1857,11 @@
       <c r="K32" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L32" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -1794,8 +1896,11 @@
       <c r="K33" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L33" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -1830,8 +1935,11 @@
       <c r="K34" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L34" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -1866,8 +1974,11 @@
       <c r="K35" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L35" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -1902,8 +2013,11 @@
       <c r="K36" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L36" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -1938,8 +2052,11 @@
       <c r="K37" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L37" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -1974,8 +2091,11 @@
       <c r="K38" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L38" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -2010,8 +2130,11 @@
       <c r="K39" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L39" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -2046,8 +2169,11 @@
       <c r="K40" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L40" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -2082,8 +2208,11 @@
       <c r="K41" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L41" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -2118,8 +2247,11 @@
       <c r="K42" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L42" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -2154,8 +2286,11 @@
       <c r="K43" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L43" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -2190,8 +2325,11 @@
       <c r="K44" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L44" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -2226,8 +2364,11 @@
       <c r="K45" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L45" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -2262,8 +2403,11 @@
       <c r="K46" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L46" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -2298,8 +2442,11 @@
       <c r="K47" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L47" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="15">
         <v>47</v>
       </c>
@@ -2334,8 +2481,11 @@
       <c r="K48" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L48" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="15">
         <v>48</v>
       </c>
@@ -2370,8 +2520,11 @@
       <c r="K49" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L49" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="15">
         <v>49</v>
       </c>
@@ -2406,8 +2559,11 @@
       <c r="K50" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L50" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="15">
         <v>50</v>
       </c>
@@ -2442,8 +2598,11 @@
       <c r="K51" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L51" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="15">
         <v>51</v>
       </c>
@@ -2478,8 +2637,11 @@
       <c r="K52" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L52" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="15">
         <v>52</v>
       </c>
@@ -2514,8 +2676,11 @@
       <c r="K53" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L53" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="15">
         <v>53</v>
       </c>
@@ -2550,8 +2715,11 @@
       <c r="K54" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L54" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="15">
         <v>54</v>
       </c>
@@ -2586,8 +2754,11 @@
       <c r="K55" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L55" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="15">
         <v>55</v>
       </c>
@@ -2622,8 +2793,11 @@
       <c r="K56" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L56" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="15">
         <v>56</v>
       </c>
@@ -2658,8 +2832,11 @@
       <c r="K57" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L57" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="15">
         <v>57</v>
       </c>
@@ -2694,8 +2871,11 @@
       <c r="K58" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L58" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="15">
         <v>58</v>
       </c>
@@ -2730,8 +2910,11 @@
       <c r="K59" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L59" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="15">
         <v>59</v>
       </c>
@@ -2766,8 +2949,11 @@
       <c r="K60" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L60" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="15">
         <v>60</v>
       </c>
@@ -2802,8 +2988,11 @@
       <c r="K61" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L61" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="15">
         <v>61</v>
       </c>
@@ -2838,8 +3027,11 @@
       <c r="K62" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L62" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="15">
         <v>62</v>
       </c>
@@ -2874,8 +3066,11 @@
       <c r="K63" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L63" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="15">
         <v>63</v>
       </c>
@@ -2910,8 +3105,11 @@
       <c r="K64" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L64" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="15">
         <v>64</v>
       </c>
@@ -2946,8 +3144,11 @@
       <c r="K65" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L65" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="15">
         <v>65</v>
       </c>
@@ -2982,8 +3183,11 @@
       <c r="K66" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L66" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="15">
         <v>66</v>
       </c>
@@ -3018,8 +3222,11 @@
       <c r="K67" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L67" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="15">
         <v>67</v>
       </c>
@@ -3054,8 +3261,11 @@
       <c r="K68" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L68" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="15">
         <v>68</v>
       </c>
@@ -3090,8 +3300,11 @@
       <c r="K69" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L69" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="15">
         <v>69</v>
       </c>
@@ -3126,8 +3339,11 @@
       <c r="K70" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L70" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="15">
         <v>70</v>
       </c>
@@ -3162,8 +3378,11 @@
       <c r="K71" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L71" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="15">
         <v>71</v>
       </c>
@@ -3198,8 +3417,11 @@
       <c r="K72" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L72" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="15">
         <v>72</v>
       </c>
@@ -3234,8 +3456,11 @@
       <c r="K73" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L73" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="15">
         <v>73</v>
       </c>
@@ -3270,8 +3495,11 @@
       <c r="K74" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L74" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="15">
         <v>74</v>
       </c>
@@ -3306,8 +3534,11 @@
       <c r="K75" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L75" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="15">
         <v>75</v>
       </c>
@@ -3342,8 +3573,11 @@
       <c r="K76" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L76" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="15">
         <v>76</v>
       </c>
@@ -3378,8 +3612,11 @@
       <c r="K77" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L77" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="15">
         <v>77</v>
       </c>
@@ -3414,8 +3651,11 @@
       <c r="K78" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L78" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="15">
         <v>78</v>
       </c>
@@ -3450,8 +3690,11 @@
       <c r="K79" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L79" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="15">
         <v>79</v>
       </c>
@@ -3486,8 +3729,11 @@
       <c r="K80" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L80" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="15">
         <v>80</v>
       </c>
@@ -3522,8 +3768,11 @@
       <c r="K81" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L81" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="15">
         <v>81</v>
       </c>
@@ -3558,8 +3807,11 @@
       <c r="K82" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L82" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="15">
         <v>82</v>
       </c>
@@ -3594,8 +3846,11 @@
       <c r="K83" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L83" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="15">
         <v>83</v>
       </c>
@@ -3630,8 +3885,11 @@
       <c r="K84" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L84" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="15">
         <v>84</v>
       </c>
@@ -3666,8 +3924,11 @@
       <c r="K85" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L85" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="15">
         <v>85</v>
       </c>
@@ -3702,8 +3963,11 @@
       <c r="K86" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L86" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="15">
         <v>86</v>
       </c>
@@ -3738,8 +4002,11 @@
       <c r="K87" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L87" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="15">
         <v>87</v>
       </c>
@@ -3774,8 +4041,11 @@
       <c r="K88" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L88" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="15">
         <v>88</v>
       </c>
@@ -3810,8 +4080,11 @@
       <c r="K89" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L89" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="15">
         <v>89</v>
       </c>
@@ -3846,8 +4119,11 @@
       <c r="K90" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L90" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="15">
         <v>90</v>
       </c>
@@ -3882,8 +4158,11 @@
       <c r="K91" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L91" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="15">
         <v>91</v>
       </c>
@@ -3918,8 +4197,11 @@
       <c r="K92" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L92" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="15">
         <v>92</v>
       </c>
@@ -3954,8 +4236,11 @@
       <c r="K93" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L93" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="15">
         <v>93</v>
       </c>
@@ -3990,8 +4275,11 @@
       <c r="K94" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L94" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="15">
         <v>94</v>
       </c>
@@ -4026,8 +4314,11 @@
       <c r="K95" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L95" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="15">
         <v>95</v>
       </c>
@@ -4062,8 +4353,11 @@
       <c r="K96" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L96" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="15">
         <v>96</v>
       </c>
@@ -4098,8 +4392,11 @@
       <c r="K97" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L97" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="15">
         <v>97</v>
       </c>
@@ -4134,8 +4431,11 @@
       <c r="K98" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L98" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="15">
         <v>98</v>
       </c>
@@ -4170,8 +4470,11 @@
       <c r="K99" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L99" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="15">
         <v>99</v>
       </c>
@@ -4206,8 +4509,11 @@
       <c r="K100" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L100" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="15">
         <v>100</v>
       </c>
@@ -4242,8 +4548,11 @@
       <c r="K101" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L101" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="15">
         <v>101</v>
       </c>
@@ -4278,8 +4587,11 @@
       <c r="K102" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L102" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="15">
         <v>102</v>
       </c>
@@ -4314,8 +4626,11 @@
       <c r="K103" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L103" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="15">
         <v>103</v>
       </c>
@@ -4350,8 +4665,11 @@
       <c r="K104" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L104" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="15">
         <v>104</v>
       </c>
@@ -4386,8 +4704,11 @@
       <c r="K105" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L105" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="15">
         <v>105</v>
       </c>
@@ -4422,8 +4743,11 @@
       <c r="K106" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L106" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="15">
         <v>106</v>
       </c>
@@ -4458,8 +4782,11 @@
       <c r="K107" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L107" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="15">
         <v>107</v>
       </c>
@@ -4494,8 +4821,11 @@
       <c r="K108" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L108" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="15">
         <v>108</v>
       </c>
@@ -4530,8 +4860,11 @@
       <c r="K109" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L109" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="15">
         <v>109</v>
       </c>
@@ -4566,8 +4899,11 @@
       <c r="K110" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L110" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="15">
         <v>110</v>
       </c>
@@ -4602,8 +4938,11 @@
       <c r="K111" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L111" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="15">
         <v>111</v>
       </c>
@@ -4638,8 +4977,11 @@
       <c r="K112" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L112" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="15">
         <v>112</v>
       </c>
@@ -4674,8 +5016,11 @@
       <c r="K113" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L113" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="15">
         <v>113</v>
       </c>
@@ -4710,8 +5055,11 @@
       <c r="K114" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L114" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="15">
         <v>114</v>
       </c>
@@ -4746,8 +5094,11 @@
       <c r="K115" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L115" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="15">
         <v>115</v>
       </c>
@@ -4782,8 +5133,11 @@
       <c r="K116" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L116" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="15">
         <v>116</v>
       </c>
@@ -4818,8 +5172,11 @@
       <c r="K117" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L117" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="15">
         <v>117</v>
       </c>
@@ -4854,8 +5211,11 @@
       <c r="K118" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L118" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="15">
         <v>118</v>
       </c>
@@ -4890,8 +5250,11 @@
       <c r="K119" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L119" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="15">
         <v>119</v>
       </c>
@@ -4926,8 +5289,11 @@
       <c r="K120" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L120" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="15">
         <v>120</v>
       </c>
@@ -4962,8 +5328,11 @@
       <c r="K121" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L121" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="15">
         <v>121</v>
       </c>
@@ -4998,8 +5367,11 @@
       <c r="K122" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L122" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="15">
         <v>122</v>
       </c>
@@ -5034,8 +5406,11 @@
       <c r="K123" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L123" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="15">
         <v>123</v>
       </c>
@@ -5070,8 +5445,11 @@
       <c r="K124" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L124" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="15">
         <v>124</v>
       </c>
@@ -5106,8 +5484,11 @@
       <c r="K125" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L125" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="15">
         <v>125</v>
       </c>
@@ -5142,8 +5523,11 @@
       <c r="K126" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L126" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="15">
         <v>126</v>
       </c>
@@ -5178,8 +5562,11 @@
       <c r="K127" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L127" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="15">
         <v>127</v>
       </c>
@@ -5214,8 +5601,11 @@
       <c r="K128" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L128" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="15">
         <v>128</v>
       </c>
@@ -5250,8 +5640,11 @@
       <c r="K129" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L129" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="15">
         <v>129</v>
       </c>
@@ -5286,8 +5679,11 @@
       <c r="K130" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L130" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="15">
         <v>130</v>
       </c>
@@ -5322,8 +5718,11 @@
       <c r="K131" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L131" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="15">
         <v>131</v>
       </c>
@@ -5358,8 +5757,11 @@
       <c r="K132" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L132" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="15">
         <v>132</v>
       </c>
@@ -5394,8 +5796,11 @@
       <c r="K133" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L133" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="15">
         <v>133</v>
       </c>
@@ -5430,8 +5835,11 @@
       <c r="K134" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L134" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="15">
         <v>134</v>
       </c>
@@ -5466,8 +5874,11 @@
       <c r="K135" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L135" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="15">
         <v>135</v>
       </c>
@@ -5502,8 +5913,11 @@
       <c r="K136" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L136" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="15">
         <v>136</v>
       </c>
@@ -5538,8 +5952,11 @@
       <c r="K137" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L137" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="15">
         <v>137</v>
       </c>
@@ -5574,8 +5991,11 @@
       <c r="K138" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L138" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="15">
         <v>138</v>
       </c>
@@ -5610,8 +6030,11 @@
       <c r="K139" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L139" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="15">
         <v>139</v>
       </c>
@@ -5646,8 +6069,11 @@
       <c r="K140" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L140" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="15">
         <v>140</v>
       </c>
@@ -5682,8 +6108,11 @@
       <c r="K141" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L141" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="15">
         <v>141</v>
       </c>
@@ -5718,8 +6147,11 @@
       <c r="K142" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L142" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="15">
         <v>142</v>
       </c>
@@ -5754,8 +6186,11 @@
       <c r="K143" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L143" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="15">
         <v>143</v>
       </c>
@@ -5790,8 +6225,11 @@
       <c r="K144" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L144" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="15">
         <v>144</v>
       </c>
@@ -5826,8 +6264,11 @@
       <c r="K145" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L145" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="15">
         <v>145</v>
       </c>
@@ -5862,8 +6303,11 @@
       <c r="K146" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L146" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="15">
         <v>146</v>
       </c>
@@ -5898,8 +6342,11 @@
       <c r="K147" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L147" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="15">
         <v>147</v>
       </c>
@@ -5934,8 +6381,11 @@
       <c r="K148" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L148" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="15">
         <v>148</v>
       </c>
@@ -5970,8 +6420,11 @@
       <c r="K149" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L149" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="15">
         <v>149</v>
       </c>
@@ -6006,8 +6459,11 @@
       <c r="K150" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L150" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="15">
         <v>150</v>
       </c>
@@ -6042,8 +6498,11 @@
       <c r="K151" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L151" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="15">
         <v>151</v>
       </c>
@@ -6078,8 +6537,11 @@
       <c r="K152" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L152" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="15">
         <v>152</v>
       </c>
@@ -6114,8 +6576,11 @@
       <c r="K153" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L153" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="15">
         <v>153</v>
       </c>
@@ -6150,8 +6615,11 @@
       <c r="K154" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L154" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="15">
         <v>154</v>
       </c>
@@ -6186,8 +6654,11 @@
       <c r="K155" s="15">
         <v>16</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="L155" s="15">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="15">
         <v>155</v>
       </c>
@@ -6221,6 +6692,9 @@
       </c>
       <c r="K156" s="15">
         <v>16</v>
+      </c>
+      <c r="L156" s="15">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>